<commit_message>
Remove duplicate codes; create fluid-category summary; list of all lab events with counts
</commit_message>
<xml_diff>
--- a/labevents/Lab-Event-Multiple-Units.xlsx
+++ b/labevents/Lab-Event-Multiple-Units.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -391,19 +391,19 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>490628</v>
+        <v>895</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>11556-8</t>
+          <t>10548-6</t>
         </is>
       </c>
       <c r="C2">
-        <v>50821</v>
+        <v>50969</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>pO2</t>
+          <t>Phenytoin, Percent Free</t>
         </is>
       </c>
       <c r="E2">
@@ -411,25 +411,25 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>mm Hg|MM HG</t>
+          <t>%|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>490594</v>
+        <v>11468</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>11557-6</t>
+          <t>10839-9</t>
         </is>
       </c>
       <c r="C3">
-        <v>50818</v>
+        <v>51002</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>pCO2</t>
+          <t>Troponin I</t>
         </is>
       </c>
       <c r="E3">
@@ -437,25 +437,25 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>mm Hg|MM HG</t>
+          <t>ng/mL|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>530752</v>
+        <v>490651</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>11558-4</t>
+          <t>11555-0</t>
         </is>
       </c>
       <c r="C4">
-        <v>50820</v>
+        <v>50802</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>pH</t>
+          <t>Base Excess</t>
         </is>
       </c>
       <c r="E4">
@@ -463,25 +463,25 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>units|UNITS</t>
+          <t>mEq/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>306</v>
+        <v>490628</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15067-2</t>
+          <t>11556-8</t>
         </is>
       </c>
       <c r="C5">
-        <v>50926</v>
+        <v>50821</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Follicle Stimulating Hormone</t>
+          <t>pO2</t>
         </is>
       </c>
       <c r="E5">
@@ -489,25 +489,25 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>mIU/L|mIU/mL</t>
+          <t>mm Hg|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>229</v>
+        <v>490594</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1599-0</t>
+          <t>11557-6</t>
         </is>
       </c>
       <c r="C6">
-        <v>50958</v>
+        <v>50818</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Luteinizing Hormone</t>
+          <t>pCO2</t>
         </is>
       </c>
       <c r="E6">
@@ -515,25 +515,25 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>mIU/L|mIU/mL</t>
+          <t>mm Hg|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>24987</v>
+        <v>530752</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1644-4</t>
+          <t>11558-4</t>
         </is>
       </c>
       <c r="C7">
-        <v>51000</v>
+        <v>50820</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Triglycerides</t>
+          <t>pH</t>
         </is>
       </c>
       <c r="E7">
@@ -541,25 +541,25 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>mg/dL|MG/DL</t>
+          <t>units|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>2779</v>
+        <v>1780</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1834-1</t>
+          <t>13438-7</t>
         </is>
       </c>
       <c r="C8">
-        <v>50864</v>
+        <v>51098</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Alpha-Fetoprotein</t>
+          <t>Prot. Electrophoresis, Urine</t>
         </is>
       </c>
       <c r="E8">
@@ -567,51 +567,51 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ng/mL|nG/ML</t>
+          <t>+/-|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>6604</v>
+        <v>2165</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1988-5</t>
+          <t>14958-3</t>
         </is>
       </c>
       <c r="C9">
-        <v>50889</v>
+        <v>51070</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>C-Reactive Protein</t>
+          <t>Albumin/Creatinine, Urine</t>
         </is>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>mg/dL|MG/DL|mg/L</t>
+          <t>mg/g|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>653</v>
+        <v>306</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2162-6</t>
+          <t>15067-2</t>
         </is>
       </c>
       <c r="C10">
-        <v>51067</v>
+        <v>50926</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>24 hr Creatinine</t>
+          <t>Follicle Stimulating Hormone</t>
         </is>
       </c>
       <c r="E10">
@@ -619,25 +619,25 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>mg/24hours|mg/24hr</t>
+          <t>mIU/mL|mIU/L</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>58</v>
+        <v>229</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2191-5</t>
+          <t>1599-0</t>
         </is>
       </c>
       <c r="C11">
-        <v>50916</v>
+        <v>50958</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>DHEA-Sulfate</t>
+          <t>Luteinizing Hormone</t>
         </is>
       </c>
       <c r="E11">
@@ -645,25 +645,25 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>nG/mL|ug/dL</t>
+          <t>mIU/mL|mIU/L</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>17946</v>
+        <v>24987</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2276-4</t>
+          <t>1644-4</t>
         </is>
       </c>
       <c r="C12">
-        <v>50924</v>
+        <v>51000</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Ferritin</t>
+          <t>Triglycerides</t>
         </is>
       </c>
       <c r="E12">
@@ -671,25 +671,25 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ng/ml|ng/mL</t>
+          <t>mg/dL|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>3280</v>
+        <v>219462</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>26457-2</t>
+          <t>1742-6</t>
         </is>
       </c>
       <c r="C13">
-        <v>51127</v>
+        <v>50861</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>RBC, Ascites</t>
+          <t>Alanine Aminotransferase (ALT)</t>
         </is>
       </c>
       <c r="E13">
@@ -697,25 +697,25 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>#/CU MM|#/uL</t>
+          <t>IU/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>3347</v>
+        <v>146694</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>26468-9</t>
+          <t>1751-7</t>
         </is>
       </c>
       <c r="C14">
-        <v>51128</v>
+        <v>50862</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>WBC, Ascites</t>
+          <t>Albumin</t>
         </is>
       </c>
       <c r="E14">
@@ -723,51 +723,51 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>#/CU MM|#/uL</t>
+          <t>g/dL|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>18816</v>
+        <v>769810</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2692-2</t>
+          <t>1863-0</t>
         </is>
       </c>
       <c r="C15">
-        <v>50964</v>
+        <v>50868</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Osmolality, Measured</t>
+          <t>Anion Gap</t>
         </is>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>mOsm/kg|MOSM/KG|MOSM/L</t>
+          <t>mEq/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>406</v>
+        <v>219452</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2842-3</t>
+          <t>1920-8</t>
         </is>
       </c>
       <c r="C16">
-        <v>50973</v>
+        <v>50878</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Prolactin</t>
+          <t>Asparate Aminotransferase (AST)</t>
         </is>
       </c>
       <c r="E16">
@@ -775,25 +775,25 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ng/mL|nG/mL</t>
+          <t>IU/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>3635</v>
+        <v>780648</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2857-1</t>
+          <t>1963-8</t>
         </is>
       </c>
       <c r="C17">
-        <v>50974</v>
+        <v>50882</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Prostate Specific Antigen</t>
+          <t>Bicarbonate</t>
         </is>
       </c>
       <c r="E17">
@@ -801,25 +801,25 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>ng/mL|ug/L</t>
+          <t>mEq/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>225</v>
+        <v>1000</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2889-4</t>
+          <t>1964-6</t>
         </is>
       </c>
       <c r="C18">
-        <v>51068</v>
+        <v>51076</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>24 hr Protein</t>
+          <t>Bicarbonate, Urine</t>
         </is>
       </c>
       <c r="E18">
@@ -827,25 +827,25 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>mg/24hours|mg/24hr</t>
+          <t>mEq/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>422</v>
+        <v>238263</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2991-8</t>
+          <t>1975-2</t>
         </is>
       </c>
       <c r="C19">
-        <v>50989</v>
+        <v>50885</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Testosterone, Free</t>
+          <t>Bilirubin, Total</t>
         </is>
       </c>
       <c r="E19">
@@ -853,51 +853,51 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>ng/dL|pg/mL</t>
+          <t>mg/dL|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>28220</v>
+        <v>6604</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3016-3</t>
+          <t>1988-5</t>
         </is>
       </c>
       <c r="C20">
-        <v>50993</v>
+        <v>50889</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Thyroid Stimulating Hormone</t>
+          <t>C-Reactive Protein</t>
         </is>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>uIU/mL|uU/ML</t>
+          <t>mg/dL|mg/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>8104</v>
+        <v>249110</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3024-7</t>
+          <t>1994-3</t>
         </is>
       </c>
       <c r="C21">
-        <v>50995</v>
+        <v>50808</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Thyroxine (T4), Free</t>
+          <t>Free Calcium</t>
         </is>
       </c>
       <c r="E21">
@@ -905,25 +905,25 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>ng/dl|ng/dL</t>
+          <t>mmol/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>3201</v>
+        <v>22016</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3026-2</t>
+          <t>19991-9</t>
         </is>
       </c>
       <c r="C22">
-        <v>50994</v>
+        <v>50801</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Thyroxine (T4)</t>
+          <t>Alveolar-arterial Gradient</t>
         </is>
       </c>
       <c r="E22">
@@ -931,25 +931,25 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ug/dL|uG/DL</t>
+          <t>&lt;missing&gt;|mm Hg</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>592</v>
+        <v>127960</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3050-2</t>
+          <t>19994-3</t>
         </is>
       </c>
       <c r="C23">
-        <v>51005</v>
+        <v>50816</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Uptake Ratio</t>
+          <t>Oxygen</t>
         </is>
       </c>
       <c r="E23">
@@ -957,25 +957,25 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Ratio|RATIO</t>
+          <t>&lt;missing&gt;|%</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2270</v>
+        <v>591932</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3053-6</t>
+          <t>2000-8</t>
         </is>
       </c>
       <c r="C24">
-        <v>51001</v>
+        <v>50893</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Triiodothyronine (T3)</t>
+          <t>Calcium, Total</t>
         </is>
       </c>
       <c r="E24">
@@ -983,25 +983,25 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>ng/dL|NG/DL</t>
+          <t>mg/dL|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>494</v>
+        <v>43</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3086-6</t>
+          <t>2023-0</t>
         </is>
       </c>
       <c r="C25">
-        <v>51105</v>
+        <v>50830</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Uric Acid, Urine</t>
+          <t>pCO2, Body Fluid</t>
         </is>
       </c>
       <c r="E25">
@@ -1009,25 +1009,25 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>mg/dL|MG/DL</t>
+          <t>&lt;missing&gt;|mm Hg</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>584</v>
+        <v>173418</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>32215-6</t>
+          <t>20564-1</t>
         </is>
       </c>
       <c r="C26">
-        <v>50896</v>
+        <v>50817</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Calculated Thyroxine (T4) Index</t>
+          <t>Oxygen Saturation</t>
         </is>
       </c>
       <c r="E26">
@@ -1035,25 +1035,25 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>ug/dL|uG/DL</t>
+          <t>&lt;missing&gt;|%</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>490641</v>
+        <v>22911</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>34728-6</t>
+          <t>20569-0</t>
         </is>
       </c>
       <c r="C27">
-        <v>50804</v>
+        <v>50908</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Calculated Total CO2</t>
+          <t>CK-MB Index</t>
         </is>
       </c>
       <c r="E27">
@@ -1061,25 +1061,25 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>mEq/L|MEQ/L</t>
+          <t>%|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>253</v>
+        <v>89715</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4049-3</t>
+          <t>20570-8</t>
         </is>
       </c>
       <c r="C28">
-        <v>50990</v>
+        <v>50810</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Theophylline</t>
+          <t>Hematocrit, Calculated</t>
         </is>
       </c>
       <c r="E28">
@@ -1087,25 +1087,25 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>ug/ml|ug/mL</t>
+          <t>%|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>11970</v>
+        <v>54728</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4542-7</t>
+          <t>20578-1</t>
         </is>
       </c>
       <c r="C29">
-        <v>50935</v>
+        <v>51009</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Haptoglobin</t>
+          <t>Vancomycin</t>
         </is>
       </c>
       <c r="E29">
@@ -1113,25 +1113,25 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>mg/dL|MG/DL</t>
+          <t>ug/mL|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>99680</v>
+        <v>48188</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5770-3</t>
+          <t>2069-3</t>
         </is>
       </c>
       <c r="C30">
-        <v>51464</v>
+        <v>50806</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Bilirubin</t>
+          <t>Chloride, Whole Blood</t>
         </is>
       </c>
       <c r="E30">
@@ -1139,25 +1139,25 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>EU/dL|mg/dL</t>
+          <t>mEq/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>101817</v>
+        <v>795480</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5818-0</t>
+          <t>2075-0</t>
         </is>
       </c>
       <c r="C31">
-        <v>51514</v>
+        <v>50902</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Urobilinogen</t>
+          <t>Chloride</t>
         </is>
       </c>
       <c r="E31">
@@ -1165,25 +1165,25 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>EU/dL|mg/dL</t>
+          <t>mEq/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>469083</v>
+        <v>9600</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5902-2</t>
+          <t>2078-4</t>
         </is>
       </c>
       <c r="C32">
-        <v>51274</v>
+        <v>51078</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>Chloride, Urine</t>
         </is>
       </c>
       <c r="E32">
@@ -1191,25 +1191,25 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>sec|SECONDS</t>
+          <t>mEq/L|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>87238</v>
+        <v>18260</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>6598-7</t>
+          <t>2085-9</t>
         </is>
       </c>
       <c r="C33">
-        <v>51003</v>
+        <v>50904</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Troponin T</t>
+          <t>Cholesterol, HDL</t>
         </is>
       </c>
       <c r="E33">
@@ -1217,33 +1217,2056 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>ng/ml|ng/mL</t>
+          <t>mg/dL|&lt;missing&gt;</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>16486</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2090-9</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>50905</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Cholesterol, LDL, Calculated</t>
+        </is>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>19444</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2093-3</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>50907</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Cholesterol, Total</t>
+        </is>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>13554</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2143-6</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>50909</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Cortisol</t>
+        </is>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>ug/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>132400</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2157-6</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>50910</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Creatine Kinase (CK)</t>
+        </is>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>IU/L|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>797389</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2160-0</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>50912</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Creatinine</t>
+        </is>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>33062</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2161-8</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>51082</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Creatinine, Urine</t>
+        </is>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>653</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2162-6</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>51067</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>24 hr Creatinine</t>
+        </is>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>mg/24hr|mg/24hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>58</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2191-5</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>50916</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>DHEA-Sulfate</t>
+        </is>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>ug/dL|ng/mL</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>196736</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2339-0</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>50809</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Glucose</t>
+        </is>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>748896</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2345-7</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>50931</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Glucose</t>
+        </is>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>664123</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2601-3</t>
+        </is>
+      </c>
+      <c r="C44">
+        <v>50960</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Magnesium</t>
+        </is>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>3280</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>26457-2</t>
+        </is>
+      </c>
+      <c r="C45">
+        <v>51127</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>RBC, Ascites</t>
+        </is>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>#/uL|#/CU MM</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>3347</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>26468-9</t>
+        </is>
+      </c>
+      <c r="C46">
+        <v>51128</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>WBC, Ascites</t>
+        </is>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>#/uL|#/CU MM</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>59158</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>26498-6</t>
+        </is>
+      </c>
+      <c r="C47">
+        <v>51255</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Myelocytes</t>
+        </is>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>18816</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2692-2</t>
+        </is>
+      </c>
+      <c r="C48">
+        <v>50964</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Osmolality, Measured</t>
+        </is>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>mOsm/kg|MOSM/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>18838</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2695-5</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>51093</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Osmolality, Urine</t>
+        </is>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>mOsm/kg|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>13</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2706-0</t>
+        </is>
+      </c>
+      <c r="C50">
+        <v>50832</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>pO2, Body Fluid</t>
+        </is>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>&lt;missing&gt;|mm Hg</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>1442</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2748-2</t>
+        </is>
+      </c>
+      <c r="C51">
+        <v>50831</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>units|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>590502</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2777-1</t>
+        </is>
+      </c>
+      <c r="C52">
+        <v>50970</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Phosphate</t>
+        </is>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2821-7</t>
+        </is>
+      </c>
+      <c r="C53">
+        <v>50833</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Potassium</t>
+        </is>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>&lt;missing&gt;|mEq/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>845737</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2823-3</t>
+        </is>
+      </c>
+      <c r="C54">
+        <v>50971</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Potassium</t>
+        </is>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>mEq/L|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>10931</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2828-2</t>
+        </is>
+      </c>
+      <c r="C55">
+        <v>51097</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Potassium, Urine</t>
+        </is>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>mEq/L|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>59206</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>28541-1</t>
+        </is>
+      </c>
+      <c r="C56">
+        <v>51251</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Metamyelocytes</t>
+        </is>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>3635</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2857-1</t>
+        </is>
+      </c>
+      <c r="C57">
+        <v>50974</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Prostate Specific Antigen</t>
+        </is>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>ng/mL|ug/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>225</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2889-4</t>
+        </is>
+      </c>
+      <c r="C58">
+        <v>51068</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>24 hr Protein</t>
+        </is>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>mg/24hr|mg/24hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>71504</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2947-0</t>
+        </is>
+      </c>
+      <c r="C59">
+        <v>50824</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Sodium, Whole Blood</t>
+        </is>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>mEq/L|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>808401</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2951-2</t>
+        </is>
+      </c>
+      <c r="C60">
+        <v>50983</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Sodium</t>
+        </is>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>mEq/L|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>25990</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2955-3</t>
+        </is>
+      </c>
+      <c r="C61">
+        <v>51100</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Sodium, Urine</t>
+        </is>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>mEq/L|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>422</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2991-8</t>
+        </is>
+      </c>
+      <c r="C62">
+        <v>50989</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Testosterone, Free</t>
+        </is>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>pg/mL|ng/dL</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>28220</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>3016-3</t>
+        </is>
+      </c>
+      <c r="C63">
+        <v>50993</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Thyroid Stimulating Hormone</t>
+        </is>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>uU/ML|uIU/mL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>8104</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>3024-7</t>
+        </is>
+      </c>
+      <c r="C64">
+        <v>50995</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Thyroxine (T4), Free</t>
+        </is>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>ng/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>18355</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>3084-1</t>
+        </is>
+      </c>
+      <c r="C65">
+        <v>51007</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Uric Acid</t>
+        </is>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>791838</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>3094-0</t>
+        </is>
+      </c>
+      <c r="C66">
+        <v>51006</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Urea Nitrogen</t>
+        </is>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>453</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>31017-7</t>
+        </is>
+      </c>
+      <c r="C67">
+        <v>50996</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Tissue Transglutaminase Ab, IgA</t>
+        </is>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>units|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>474930</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>3173-2</t>
+        </is>
+      </c>
+      <c r="C68">
+        <v>51275</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>PTT</t>
+        </is>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>sec|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>15</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>3240-9</t>
+        </is>
+      </c>
+      <c r="C69">
+        <v>51211</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Factor XIII</t>
+        </is>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
+        <v>187116</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>32693-4</t>
+        </is>
+      </c>
+      <c r="C70">
+        <v>50813</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Lactate</t>
+        </is>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>mmol/L|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>6943</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>33762-6</t>
+        </is>
+      </c>
+      <c r="C71">
+        <v>50963</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>NTproBNP</t>
+        </is>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>pg/mL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>490641</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>34728-6</t>
+        </is>
+      </c>
+      <c r="C72">
+        <v>50804</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Calculated Total CO2</t>
+        </is>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>mEq/L|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>960</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>3969-3</t>
+        </is>
+      </c>
+      <c r="C73">
+        <v>50968</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Phenytoin, Free</t>
+        </is>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>ug/mL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>881764</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>4544-3</t>
+        </is>
+      </c>
+      <c r="C74">
+        <v>51221</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Hematocrit</t>
+        </is>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>4476</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>48065-7</t>
+        </is>
+      </c>
+      <c r="C75">
+        <v>51196</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>D-Dimer</t>
+        </is>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>ng/mL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>1494</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>5183-9</t>
+        </is>
+      </c>
+      <c r="C76">
+        <v>50937</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Hepatitis A Virus Antibody</t>
+        </is>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Pos/Neg|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77">
+        <v>266</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>5380-1</t>
+        </is>
+      </c>
+      <c r="C77">
+        <v>50877</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Anti-Thyroglobulin Antibodies</t>
+        </is>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>IU/mL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>99680</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>5770-3</t>
+        </is>
+      </c>
+      <c r="C78">
+        <v>51464</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Bilirubin</t>
+        </is>
+      </c>
+      <c r="E78">
+        <v>3</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>EU/dL|mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>83200</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>5787-7</t>
+        </is>
+      </c>
+      <c r="C79">
+        <v>51476</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Epithelial Cells</t>
+        </is>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>#/hpf|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>101280</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>5792-7</t>
+        </is>
+      </c>
+      <c r="C80">
+        <v>51478</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Glucose</t>
+        </is>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>99726</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>5794-3</t>
+        </is>
+      </c>
+      <c r="C81">
+        <v>51466</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Blood</t>
+        </is>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>101624</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>5797-6</t>
+        </is>
+      </c>
+      <c r="C82">
+        <v>51484</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Ketone</t>
+        </is>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>116081</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>5803-2</t>
+        </is>
+      </c>
+      <c r="C83">
+        <v>51491</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>units|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>106412</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>5804-0</t>
+        </is>
+      </c>
+      <c r="C84">
+        <v>51492</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Protein</t>
+        </is>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>84278</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>5808-1</t>
+        </is>
+      </c>
+      <c r="C85">
+        <v>51493</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>RBC</t>
+        </is>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>#/hpf|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>115858</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>5811-5</t>
+        </is>
+      </c>
+      <c r="C86">
+        <v>51498</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Specific Gravity</t>
+        </is>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> |&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>101817</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>5818-0</t>
+        </is>
+      </c>
+      <c r="C87">
+        <v>51514</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Urobilinogen</t>
+        </is>
+      </c>
+      <c r="E87">
+        <v>3</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>EU/dL|mg/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>84682</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>5821-4</t>
+        </is>
+      </c>
+      <c r="C88">
+        <v>51516</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>WBC</t>
+        </is>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>#/hpf|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>469083</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>5902-2</t>
+        </is>
+      </c>
+      <c r="C89">
+        <v>51274</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>sec|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>192949</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>6298-4</t>
+        </is>
+      </c>
+      <c r="C90">
+        <v>50822</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Potassium, Whole Blood</t>
+        </is>
+      </c>
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>mEq/L|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>207847</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>6768-6</t>
+        </is>
+      </c>
+      <c r="C91">
+        <v>50863</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Alkaline Phosphatase</t>
+        </is>
+      </c>
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>IU/L|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>115802</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>6773-6</t>
+        </is>
+      </c>
+      <c r="C92">
+        <v>50911</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Creatine Kinase, MB Isoenzyme</t>
+        </is>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>ng/mL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
         <v>834</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B93" t="inlineStr">
         <is>
           <t>6928-6</t>
         </is>
       </c>
-      <c r="C34">
+      <c r="C93">
         <v>50980</v>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D93" t="inlineStr">
         <is>
           <t>Rheumatoid Factor</t>
         </is>
       </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>I.U.|IU/mL</t>
+      <c r="E93">
+        <v>2</v>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>IU/mL|I.U.</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>172124</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>704-7</t>
+        </is>
+      </c>
+      <c r="C94">
+        <v>51146</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Basophils</t>
+        </is>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>172126</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>711-2</t>
+        </is>
+      </c>
+      <c r="C95">
+        <v>51200</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Eosinophils</t>
+        </is>
+      </c>
+      <c r="E95">
+        <v>2</v>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>89712</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>718-7</t>
+        </is>
+      </c>
+      <c r="C96">
+        <v>50811</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Hemoglobin</t>
+        </is>
+      </c>
+      <c r="E96">
+        <v>2</v>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>g/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>752444</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>718-7</t>
+        </is>
+      </c>
+      <c r="C97">
+        <v>51222</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Hemoglobin</t>
+        </is>
+      </c>
+      <c r="E97">
+        <v>2</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>g/dL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>172131</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>731-0</t>
+        </is>
+      </c>
+      <c r="C98">
+        <v>51244</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Lymphocytes</t>
+        </is>
+      </c>
+      <c r="E98">
+        <v>2</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99">
+        <v>59334</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>733-6</t>
+        </is>
+      </c>
+      <c r="C99">
+        <v>51143</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Atypical Lymphocytes</t>
+        </is>
+      </c>
+      <c r="E99">
+        <v>2</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>172130</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>742-7</t>
+        </is>
+      </c>
+      <c r="C100">
+        <v>51254</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Monocytes</t>
+        </is>
+      </c>
+      <c r="E100">
+        <v>2</v>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>172131</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>761-7</t>
+        </is>
+      </c>
+      <c r="C101">
+        <v>51256</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Neutrophils</t>
+        </is>
+      </c>
+      <c r="E101">
+        <v>2</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102">
+        <v>75587</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>763-3</t>
+        </is>
+      </c>
+      <c r="C102">
+        <v>51144</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Bands</t>
+        </is>
+      </c>
+      <c r="E102">
+        <v>2</v>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103">
+        <v>778365</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>777-3</t>
+        </is>
+      </c>
+      <c r="C103">
+        <v>51265</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Platelet Count</t>
+        </is>
+      </c>
+      <c r="E103">
+        <v>2</v>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>K/uL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104">
+        <v>747994</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>785-6</t>
+        </is>
+      </c>
+      <c r="C104">
+        <v>51248</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>MCH</t>
+        </is>
+      </c>
+      <c r="E104">
+        <v>2</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>pg|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105">
+        <v>748147</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>786-4</t>
+        </is>
+      </c>
+      <c r="C105">
+        <v>51249</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>MCHC</t>
+        </is>
+      </c>
+      <c r="E105">
+        <v>2</v>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>747977</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>787-2</t>
+        </is>
+      </c>
+      <c r="C106">
+        <v>51250</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>MCV</t>
+        </is>
+      </c>
+      <c r="E106">
+        <v>2</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>fL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107">
+        <v>746817</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>788-0</t>
+        </is>
+      </c>
+      <c r="C107">
+        <v>51277</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>RDW</t>
+        </is>
+      </c>
+      <c r="E107">
+        <v>2</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>%|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108">
+        <v>747999</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>789-8</t>
+        </is>
+      </c>
+      <c r="C108">
+        <v>51279</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Red Blood Cells</t>
+        </is>
+      </c>
+      <c r="E108">
+        <v>2</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>m/uL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109">
+        <v>753221</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>804-5</t>
+        </is>
+      </c>
+      <c r="C109">
+        <v>51301</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>White Blood Cells</t>
+        </is>
+      </c>
+      <c r="E109">
+        <v>2</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>K/uL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110">
+        <v>160</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>8099-4</t>
+        </is>
+      </c>
+      <c r="C110">
+        <v>50992</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Thyroid Peroxidase Antibodies</t>
+        </is>
+      </c>
+      <c r="E110">
+        <v>2</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>IU/mL|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111">
+        <v>18128</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>9322-9</t>
+        </is>
+      </c>
+      <c r="C111">
+        <v>50903</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Cholesterol Ratio (Total/HDL)</t>
+        </is>
+      </c>
+      <c r="E111">
+        <v>2</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Ratio|&lt;missing&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112">
+        <v>238</v>
+      </c>
+      <c r="C112">
+        <v>51406</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>CD34</t>
+        </is>
+      </c>
+      <c r="E112">
+        <v>2</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>&lt;missing&gt;|#/uL</t>
         </is>
       </c>
     </row>

</xml_diff>